<commit_message>
added more info in regards dataset
</commit_message>
<xml_diff>
--- a/data/sythesized2.xlsx
+++ b/data/sythesized2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1b01\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D83EFE3E-26EB-481A-A04C-07831AB76A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBFC43C2-66CA-465B-9947-246FC3EB04A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="253">
+  <si>
+    <t>Countries</t>
+  </si>
   <si>
     <t>Total Spending</t>
   </si>
@@ -1635,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E498"/>
+  <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+      <selection activeCell="A250" sqref="A250:XFD250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1650,22 +1653,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>112750202</v>
@@ -1682,7 +1688,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>171844362</v>
@@ -1699,7 +1705,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>104346364</v>
@@ -1716,7 +1722,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>68241318</v>
@@ -1733,7 +1739,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>34195364</v>
@@ -1750,7 +1756,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>134238338</v>
@@ -1767,7 +1773,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
         <v>136442542</v>
@@ -1784,7 +1790,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1">
         <v>26530832</v>
@@ -1801,7 +1807,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
         <v>171791222</v>
@@ -1818,7 +1824,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
         <v>107515200</v>
@@ -1835,7 +1841,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1">
         <v>98443600</v>
@@ -1852,7 +1858,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <v>15557128</v>
@@ -1869,7 +1875,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1">
         <v>171507615</v>
@@ -1886,7 +1892,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>119452268</v>
@@ -1903,7 +1909,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1">
         <v>86387304</v>
@@ -1920,7 +1926,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
         <v>149576898</v>
@@ -1937,7 +1943,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
         <v>64506427</v>
@@ -1954,7 +1960,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
         <v>79414386</v>
@@ -1971,7 +1977,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1">
         <v>148528794</v>
@@ -1988,7 +1994,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
         <v>31527600</v>
@@ -2005,7 +2011,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>24384696</v>
@@ -2022,7 +2028,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>94037832</v>
@@ -2039,7 +2045,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>54522153</v>
@@ -2056,7 +2062,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1">
         <v>82192937</v>
@@ -2073,7 +2079,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1">
         <v>82418235</v>
@@ -2090,7 +2096,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1">
         <v>77275714</v>
@@ -2107,7 +2113,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1">
         <v>182133189</v>
@@ -2124,7 +2130,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1">
         <v>34494923</v>
@@ -2141,7 +2147,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1">
         <v>167959267</v>
@@ -2158,7 +2164,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1">
         <v>78907396</v>
@@ -2175,7 +2181,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1">
         <v>42099894</v>
@@ -2192,7 +2198,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1">
         <v>19304694</v>
@@ -2209,7 +2215,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1">
         <v>95332070</v>
@@ -2226,7 +2232,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1">
         <v>179398373</v>
@@ -2243,7 +2249,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1">
         <v>156055832</v>
@@ -2260,7 +2266,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1">
         <v>89650591</v>
@@ -2277,7 +2283,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1">
         <v>23182219</v>
@@ -2294,7 +2300,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1">
         <v>161122989</v>
@@ -2311,7 +2317,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1">
         <v>28294869</v>
@@ -2328,7 +2334,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1">
         <v>61581823</v>
@@ -2345,7 +2351,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1">
         <v>174999866</v>
@@ -2362,7 +2368,7 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" s="1">
         <v>42203540</v>
@@ -2379,7 +2385,7 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1">
         <v>39687507</v>
@@ -2396,7 +2402,7 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45" s="1">
         <v>118054299</v>
@@ -2413,7 +2419,7 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46" s="1">
         <v>124562771</v>
@@ -2430,7 +2436,7 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1">
         <v>155212026</v>
@@ -2447,7 +2453,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48" s="1">
         <v>52652020</v>
@@ -2464,7 +2470,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" s="1">
         <v>43426725</v>
@@ -2481,7 +2487,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50" s="1">
         <v>166787668</v>
@@ -2498,7 +2504,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" s="1">
         <v>60109767</v>
@@ -2515,7 +2521,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B52" s="1">
         <v>148204470</v>
@@ -2532,7 +2538,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B53" s="1">
         <v>162645151</v>
@@ -2549,7 +2555,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B54" s="1">
         <v>158973091</v>
@@ -2566,7 +2572,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B55" s="1">
         <v>22087675</v>
@@ -2583,7 +2589,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B56" s="1">
         <v>44323658</v>
@@ -2600,7 +2606,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B57" s="1">
         <v>103091665</v>
@@ -2617,7 +2623,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B58" s="1">
         <v>152158474</v>
@@ -2634,7 +2640,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B59" s="1">
         <v>177179970</v>
@@ -2651,7 +2657,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B60" s="1">
         <v>103282617</v>
@@ -2668,7 +2674,7 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B61" s="1">
         <v>33141376</v>
@@ -2685,7 +2691,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B62" s="1">
         <v>74519951</v>
@@ -2702,7 +2708,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B63" s="1">
         <v>121977645</v>
@@ -2719,7 +2725,7 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B64" s="1">
         <v>145705261</v>
@@ -2736,7 +2742,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B65" s="1">
         <v>157475334</v>
@@ -2753,7 +2759,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B66" s="1">
         <v>159773038</v>
@@ -2770,7 +2776,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B67" s="1">
         <v>162614907</v>
@@ -2787,7 +2793,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B68" s="1">
         <v>64517258</v>
@@ -2804,7 +2810,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B69" s="1">
         <v>167565525</v>
@@ -2821,7 +2827,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B70" s="1">
         <v>151814748</v>
@@ -2838,7 +2844,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B71" s="1">
         <v>186153062</v>
@@ -2855,7 +2861,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B72" s="1">
         <v>146714972</v>
@@ -2872,7 +2878,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B73" s="1">
         <v>150298096</v>
@@ -2889,7 +2895,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B74" s="1">
         <v>71729638</v>
@@ -2906,7 +2912,7 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B75" s="1">
         <v>121915784</v>
@@ -2923,7 +2929,7 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B76" s="1">
         <v>49729359</v>
@@ -2940,7 +2946,7 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B77" s="1">
         <v>38070277</v>
@@ -2957,7 +2963,7 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B78" s="1">
         <v>188419435</v>
@@ -2974,7 +2980,7 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B79" s="1">
         <v>112804459</v>
@@ -2991,7 +2997,7 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B80" s="1">
         <v>172196561</v>
@@ -3008,7 +3014,7 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B81" s="1">
         <v>137725004</v>
@@ -3025,7 +3031,7 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B82" s="1">
         <v>66439031</v>
@@ -3042,7 +3048,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B83" s="1">
         <v>161679228</v>
@@ -3059,7 +3065,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B84" s="1">
         <v>138138818</v>
@@ -3076,7 +3082,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B85" s="1">
         <v>73637565</v>
@@ -3093,7 +3099,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B86" s="1">
         <v>48680777</v>
@@ -3110,7 +3116,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B87" s="1">
         <v>163804092</v>
@@ -3127,7 +3133,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B88" s="1">
         <v>140043784</v>
@@ -3144,7 +3150,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B89" s="1">
         <v>29232549</v>
@@ -3161,7 +3167,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B90" s="1">
         <v>155469029</v>
@@ -3178,7 +3184,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B91" s="1">
         <v>109321514</v>
@@ -3195,7 +3201,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B92" s="1">
         <v>106949171</v>
@@ -3212,7 +3218,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B93" s="1">
         <v>8286733</v>
@@ -3229,7 +3235,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B94" s="1">
         <v>129702390</v>
@@ -3246,7 +3252,7 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B95" s="1">
         <v>114940005</v>
@@ -3263,7 +3269,7 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B96" s="1">
         <v>8739843</v>
@@ -3280,7 +3286,7 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B97" s="1">
         <v>152934833</v>
@@ -3297,7 +3303,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B98" s="1">
         <v>122921076</v>
@@ -3314,7 +3320,7 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B99" s="1">
         <v>96058589</v>
@@ -3331,7 +3337,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B100" s="1">
         <v>24758768</v>
@@ -3348,7 +3354,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B101" s="1">
         <v>36180342</v>
@@ -3365,7 +3371,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B102" s="1">
         <v>39733327</v>
@@ -3382,7 +3388,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B103" s="1">
         <v>151929154</v>
@@ -3399,7 +3405,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B104" s="1">
         <v>12518562</v>
@@ -3416,7 +3422,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B105" s="1">
         <v>123346660</v>
@@ -3433,7 +3439,7 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B106" s="1">
         <v>183182690</v>
@@ -3450,7 +3456,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B107" s="1">
         <v>175550302</v>
@@ -3467,7 +3473,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B108" s="1">
         <v>123585945</v>
@@ -3484,7 +3490,7 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B109" s="1">
         <v>105650426</v>
@@ -3501,7 +3507,7 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B110" s="1">
         <v>44684362</v>
@@ -3518,7 +3524,7 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B111" s="1">
         <v>170061166</v>
@@ -3535,7 +3541,7 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B112" s="1">
         <v>49462373</v>
@@ -3552,7 +3558,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B113" s="1">
         <v>44738403</v>
@@ -3569,7 +3575,7 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B114" s="1">
         <v>40176536</v>
@@ -3586,7 +3592,7 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B115" s="1">
         <v>9745668</v>
@@ -3603,7 +3609,7 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B116" s="1">
         <v>177040091</v>
@@ -3620,7 +3626,7 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B117" s="1">
         <v>51075877</v>
@@ -3637,7 +3643,7 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B118" s="1">
         <v>7158241</v>
@@ -3654,7 +3660,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B119" s="1">
         <v>172315901</v>
@@ -3671,7 +3677,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B120" s="1">
         <v>107146209</v>
@@ -3688,7 +3694,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B121" s="1">
         <v>48795052</v>
@@ -3705,7 +3711,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B122" s="1">
         <v>15571979</v>
@@ -3722,7 +3728,7 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B123" s="1">
         <v>78168706</v>
@@ -3739,7 +3745,7 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B124" s="1">
         <v>55835292</v>
@@ -3756,7 +3762,7 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B125" s="1">
         <v>32188312</v>
@@ -3773,7 +3779,7 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B126" s="1">
         <v>150631274</v>
@@ -3790,7 +3796,7 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B127" s="1">
         <v>141504809</v>
@@ -3807,7 +3813,7 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B128" s="1">
         <v>157117583</v>
@@ -3824,7 +3830,7 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B129" s="1">
         <v>38677091</v>
@@ -3841,7 +3847,7 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B130" s="1">
         <v>62522441</v>
@@ -3858,7 +3864,7 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B131" s="1">
         <v>53692160</v>
@@ -3875,7 +3881,7 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B132" s="1">
         <v>66467103</v>
@@ -3892,7 +3898,7 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B133" s="1">
         <v>4994992</v>
@@ -3909,7 +3915,7 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B134" s="1">
         <v>154356885</v>
@@ -3926,7 +3932,7 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B135" s="1">
         <v>61953960</v>
@@ -3943,7 +3949,7 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B136" s="1">
         <v>182429070</v>
@@ -3960,7 +3966,7 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B137" s="1">
         <v>167459924</v>
@@ -3977,7 +3983,7 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B138" s="1">
         <v>16332069</v>
@@ -3994,7 +4000,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B139" s="1">
         <v>31029162</v>
@@ -4011,7 +4017,7 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B140" s="1">
         <v>110749774</v>
@@ -4028,7 +4034,7 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B141" s="1">
         <v>165925961</v>
@@ -4045,7 +4051,7 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B142" s="1">
         <v>34313663</v>
@@ -4062,7 +4068,7 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B143" s="1">
         <v>51068992</v>
@@ -4079,7 +4085,7 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B144" s="1">
         <v>176721010</v>
@@ -4096,7 +4102,7 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B145" s="1">
         <v>98651644</v>
@@ -4113,7 +4119,7 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B146" s="1">
         <v>137904261</v>
@@ -4130,7 +4136,7 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B147" s="1">
         <v>113510716</v>
@@ -4147,7 +4153,7 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B148" s="1">
         <v>109632193</v>
@@ -4164,7 +4170,7 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B149" s="1">
         <v>88014411</v>
@@ -4181,7 +4187,7 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B150" s="1">
         <v>161711416</v>
@@ -4198,7 +4204,7 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B151" s="1">
         <v>30576799</v>
@@ -4215,7 +4221,7 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B152" s="1">
         <v>46964761</v>
@@ -4232,7 +4238,7 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B153" s="1">
         <v>3961234</v>
@@ -4249,7 +4255,7 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B154" s="1">
         <v>131358326</v>
@@ -4266,7 +4272,7 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B155" s="1">
         <v>168673156</v>
@@ -4283,7 +4289,7 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B156" s="1">
         <v>165120871</v>
@@ -4300,7 +4306,7 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B157" s="1">
         <v>108329185</v>
@@ -4317,7 +4323,7 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B158" s="1">
         <v>58482279</v>
@@ -4334,7 +4340,7 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B159" s="1">
         <v>54511928</v>
@@ -4351,7 +4357,7 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B160" s="1">
         <v>180169249</v>
@@ -4368,7 +4374,7 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B161" s="1">
         <v>79580595</v>
@@ -4385,7 +4391,7 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B162" s="1">
         <v>144535949</v>
@@ -4402,7 +4408,7 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B163" s="1">
         <v>179423567</v>
@@ -4419,7 +4425,7 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B164" s="1">
         <v>57770268</v>
@@ -4436,7 +4442,7 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B165" s="1">
         <v>147331405</v>
@@ -4453,7 +4459,7 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B166" s="1">
         <v>55602738</v>
@@ -4470,7 +4476,7 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B167" s="1">
         <v>127911511</v>
@@ -4487,7 +4493,7 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B168" s="1">
         <v>69615077</v>
@@ -4504,7 +4510,7 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B169" s="1">
         <v>102759299</v>
@@ -4521,7 +4527,7 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B170" s="1">
         <v>23606959</v>
@@ -4538,7 +4544,7 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B171" s="1">
         <v>166709214</v>
@@ -4555,7 +4561,7 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B172" s="1">
         <v>11925344</v>
@@ -4572,7 +4578,7 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B173" s="1">
         <v>30144408</v>
@@ -4589,7 +4595,7 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B174" s="1">
         <v>106827067</v>
@@ -4606,7 +4612,7 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B175" s="1">
         <v>76856741</v>
@@ -4623,7 +4629,7 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B176" s="1">
         <v>164182345</v>
@@ -4640,7 +4646,7 @@
     </row>
     <row r="177" spans="1:5">
       <c r="A177" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B177" s="1">
         <v>101556819</v>
@@ -4657,7 +4663,7 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B178" s="1">
         <v>43961591</v>
@@ -4674,7 +4680,7 @@
     </row>
     <row r="179" spans="1:5">
       <c r="A179" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B179" s="1">
         <v>91852203</v>
@@ -4691,7 +4697,7 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B180" s="1">
         <v>42262705</v>
@@ -4708,7 +4714,7 @@
     </row>
     <row r="181" spans="1:5">
       <c r="A181" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B181" s="1">
         <v>66893768</v>
@@ -4725,7 +4731,7 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B182" s="1">
         <v>85396907</v>
@@ -4742,7 +4748,7 @@
     </row>
     <row r="183" spans="1:5">
       <c r="A183" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B183" s="1">
         <v>56763727</v>
@@ -4759,7 +4765,7 @@
     </row>
     <row r="184" spans="1:5">
       <c r="A184" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B184" s="1">
         <v>22561370</v>
@@ -4776,7 +4782,7 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B185" s="1">
         <v>169735270</v>
@@ -4793,7 +4799,7 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B186" s="1">
         <v>95455169</v>
@@ -4810,7 +4816,7 @@
     </row>
     <row r="187" spans="1:5">
       <c r="A187" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B187" s="1">
         <v>95322453</v>
@@ -4827,7 +4833,7 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B188" s="1">
         <v>145584076</v>
@@ -4844,7 +4850,7 @@
     </row>
     <row r="189" spans="1:5">
       <c r="A189" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B189" s="1">
         <v>82095994</v>
@@ -4861,7 +4867,7 @@
     </row>
     <row r="190" spans="1:5">
       <c r="A190" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B190" s="1">
         <v>38436660</v>
@@ -4878,7 +4884,7 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B191" s="1">
         <v>132691155</v>
@@ -4895,7 +4901,7 @@
     </row>
     <row r="192" spans="1:5">
       <c r="A192" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B192" s="1">
         <v>5783344</v>
@@ -4912,7 +4918,7 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B193" s="1">
         <v>135212752</v>
@@ -4929,7 +4935,7 @@
     </row>
     <row r="194" spans="1:5">
       <c r="A194" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B194" s="1">
         <v>134490875</v>
@@ -4946,7 +4952,7 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B195" s="1">
         <v>60685103</v>
@@ -4963,7 +4969,7 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B196" s="1">
         <v>161189830</v>
@@ -4980,7 +4986,7 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B197" s="1">
         <v>70926398</v>
@@ -4997,7 +5003,7 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B198" s="1">
         <v>120626620</v>
@@ -5014,7 +5020,7 @@
     </row>
     <row r="199" spans="1:5">
       <c r="A199" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B199" s="1">
         <v>132235310</v>
@@ -5031,7 +5037,7 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B200" s="1">
         <v>119011624</v>
@@ -5048,7 +5054,7 @@
     </row>
     <row r="201" spans="1:5">
       <c r="A201" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B201" s="1">
         <v>159913964</v>
@@ -5065,7 +5071,7 @@
     </row>
     <row r="202" spans="1:5">
       <c r="A202" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B202" s="1">
         <v>57398521</v>
@@ -5082,7 +5088,7 @@
     </row>
     <row r="203" spans="1:5">
       <c r="A203" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B203" s="1">
         <v>174189831</v>
@@ -5099,7 +5105,7 @@
     </row>
     <row r="204" spans="1:5">
       <c r="A204" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B204" s="1">
         <v>18237565</v>
@@ -5116,7 +5122,7 @@
     </row>
     <row r="205" spans="1:5">
       <c r="A205" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B205" s="1">
         <v>103148933</v>
@@ -5133,7 +5139,7 @@
     </row>
     <row r="206" spans="1:5">
       <c r="A206" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B206" s="1">
         <v>170227548</v>
@@ -5150,7 +5156,7 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B207" s="1">
         <v>72679442</v>
@@ -5167,7 +5173,7 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B208" s="1">
         <v>125794425</v>
@@ -5184,7 +5190,7 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B209" s="1">
         <v>96201565</v>
@@ -5201,7 +5207,7 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B210" s="1">
         <v>141217443</v>
@@ -5218,7 +5224,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B211" s="1">
         <v>102385016</v>
@@ -5235,7 +5241,7 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B212" s="1">
         <v>143416263</v>
@@ -5252,7 +5258,7 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B213" s="1">
         <v>105025424</v>
@@ -5269,7 +5275,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B214" s="1">
         <v>163571159</v>
@@ -5286,7 +5292,7 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B215" s="1">
         <v>186681461</v>
@@ -5303,7 +5309,7 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B216" s="1">
         <v>25103960</v>
@@ -5320,7 +5326,7 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B217" s="1">
         <v>50611061</v>
@@ -5337,7 +5343,7 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B218" s="1">
         <v>29408106</v>
@@ -5354,7 +5360,7 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B219" s="1">
         <v>144093051</v>
@@ -5371,7 +5377,7 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B220" s="1">
         <v>184448754</v>
@@ -5388,7 +5394,7 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B221" s="1">
         <v>72235806</v>
@@ -5405,7 +5411,7 @@
     </row>
     <row r="222" spans="1:5">
       <c r="A222" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B222" s="1">
         <v>58876571</v>
@@ -5422,7 +5428,7 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B223" s="1">
         <v>23576398</v>
@@ -5439,7 +5445,7 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B224" s="1">
         <v>103151861</v>
@@ -5456,7 +5462,7 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B225" s="1">
         <v>5165764</v>
@@ -5473,7 +5479,7 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B226" s="1">
         <v>5426504</v>
@@ -5490,7 +5496,7 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B227" s="1">
         <v>101542108</v>
@@ -5507,7 +5513,7 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B228" s="1">
         <v>24329470</v>
@@ -5524,7 +5530,7 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B229" s="1">
         <v>51225507</v>
@@ -5541,7 +5547,7 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B230" s="1">
         <v>147433635</v>
@@ -5558,7 +5564,7 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B231" s="1">
         <v>53503282</v>
@@ -5575,7 +5581,7 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B232" s="1">
         <v>124758760</v>
@@ -5592,7 +5598,7 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B233" s="1">
         <v>58098293</v>
@@ -5609,7 +5615,7 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B234" s="1">
         <v>131541079</v>
@@ -5626,7 +5632,7 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B235" s="1">
         <v>90431504</v>
@@ -5643,7 +5649,7 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B236" s="1">
         <v>170691088</v>
@@ -5660,7 +5666,7 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B237" s="1">
         <v>84481762</v>
@@ -5677,7 +5683,7 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B238" s="1">
         <v>155640311</v>
@@ -5694,7 +5700,7 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B239" s="1">
         <v>181533393</v>
@@ -5711,7 +5717,7 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B240" s="1">
         <v>3423662</v>
@@ -5728,7 +5734,7 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B241" s="1">
         <v>114051644</v>
@@ -5745,7 +5751,7 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B242" s="1">
         <v>120301799</v>
@@ -5762,7 +5768,7 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B243" s="1">
         <v>82941173</v>
@@ -5779,7 +5785,7 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B244" s="1">
         <v>166473137</v>
@@ -5796,7 +5802,7 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B245" s="1">
         <v>44593106</v>
@@ -5813,7 +5819,7 @@
     </row>
     <row r="246" spans="1:5">
       <c r="A246" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B246" s="1">
         <v>32230518</v>
@@ -5830,7 +5836,7 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B247" s="1">
         <v>167926032</v>
@@ -5847,7 +5853,7 @@
     </row>
     <row r="248" spans="1:5">
       <c r="A248" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B248" s="1">
         <v>121122799</v>
@@ -5864,7 +5870,7 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B249" s="1">
         <v>29552468</v>
@@ -5876,1995 +5882,6 @@
         <v>29</v>
       </c>
       <c r="E249">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5">
-      <c r="B250" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5">
-      <c r="A251" t="s">
-        <v>4</v>
-      </c>
-      <c r="B251" s="1">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5">
-      <c r="A252" t="s">
-        <v>5</v>
-      </c>
-      <c r="B252" s="1">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5">
-      <c r="A253" t="s">
-        <v>6</v>
-      </c>
-      <c r="B253" s="1">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5">
-      <c r="A254" t="s">
-        <v>7</v>
-      </c>
-      <c r="B254" s="1">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5">
-      <c r="A255" t="s">
-        <v>8</v>
-      </c>
-      <c r="B255" s="1">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5">
-      <c r="A256" t="s">
-        <v>9</v>
-      </c>
-      <c r="B256" s="1">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2">
-      <c r="A257" t="s">
-        <v>10</v>
-      </c>
-      <c r="B257" s="1">
-        <v>1469</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2">
-      <c r="A258" t="s">
-        <v>11</v>
-      </c>
-      <c r="B258" s="1">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2">
-      <c r="A259" t="s">
-        <v>12</v>
-      </c>
-      <c r="B259" s="1">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2">
-      <c r="A260" t="s">
-        <v>13</v>
-      </c>
-      <c r="B260" s="1">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2">
-      <c r="A261" t="s">
-        <v>14</v>
-      </c>
-      <c r="B261" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2">
-      <c r="A262" t="s">
-        <v>15</v>
-      </c>
-      <c r="B262" s="1">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2">
-      <c r="A263" t="s">
-        <v>16</v>
-      </c>
-      <c r="B263" s="1">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2">
-      <c r="A264" t="s">
-        <v>17</v>
-      </c>
-      <c r="B264" s="1">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2">
-      <c r="A265" t="s">
-        <v>18</v>
-      </c>
-      <c r="B265" s="1">
-        <v>1739</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2">
-      <c r="A266" t="s">
-        <v>19</v>
-      </c>
-      <c r="B266" s="1">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2">
-      <c r="A267" t="s">
-        <v>20</v>
-      </c>
-      <c r="B267" s="1">
-        <v>1796</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2">
-      <c r="A268" t="s">
-        <v>21</v>
-      </c>
-      <c r="B268" s="1">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2">
-      <c r="A269" t="s">
-        <v>22</v>
-      </c>
-      <c r="B269" s="1">
-        <v>1289</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2">
-      <c r="A270" t="s">
-        <v>23</v>
-      </c>
-      <c r="B270" s="1">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2">
-      <c r="A271" t="s">
-        <v>24</v>
-      </c>
-      <c r="B271" s="1">
-        <v>1491</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2">
-      <c r="A272" t="s">
-        <v>25</v>
-      </c>
-      <c r="B272" s="1">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2">
-      <c r="A273" t="s">
-        <v>26</v>
-      </c>
-      <c r="B273" s="1">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2">
-      <c r="A274" t="s">
-        <v>27</v>
-      </c>
-      <c r="B274" s="1">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2">
-      <c r="A275" t="s">
-        <v>28</v>
-      </c>
-      <c r="B275" s="1">
-        <v>1273</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2">
-      <c r="A276" t="s">
-        <v>29</v>
-      </c>
-      <c r="B276" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2">
-      <c r="A277" t="s">
-        <v>30</v>
-      </c>
-      <c r="B277" s="1">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2">
-      <c r="A278" t="s">
-        <v>31</v>
-      </c>
-      <c r="B278" s="1">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2">
-      <c r="A279" t="s">
-        <v>32</v>
-      </c>
-      <c r="B279" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2">
-      <c r="A280" t="s">
-        <v>33</v>
-      </c>
-      <c r="B280" s="1">
-        <v>1931</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2">
-      <c r="A281" t="s">
-        <v>34</v>
-      </c>
-      <c r="B281" s="1">
-        <v>1448</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2">
-      <c r="A282" t="s">
-        <v>35</v>
-      </c>
-      <c r="B282" s="1">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2">
-      <c r="A283" t="s">
-        <v>36</v>
-      </c>
-      <c r="B283" s="1">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2">
-      <c r="A284" t="s">
-        <v>37</v>
-      </c>
-      <c r="B284" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2">
-      <c r="A285" t="s">
-        <v>38</v>
-      </c>
-      <c r="B285" s="1">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2">
-      <c r="A286" t="s">
-        <v>39</v>
-      </c>
-      <c r="B286" s="1">
-        <v>1241</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2">
-      <c r="A287" t="s">
-        <v>40</v>
-      </c>
-      <c r="B287" s="1">
-        <v>1213</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2">
-      <c r="A288" t="s">
-        <v>41</v>
-      </c>
-      <c r="B288" s="1">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2">
-      <c r="A289" t="s">
-        <v>42</v>
-      </c>
-      <c r="B289" s="1">
-        <v>1632</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2">
-      <c r="A290" t="s">
-        <v>43</v>
-      </c>
-      <c r="B290" s="1">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2">
-      <c r="A291" t="s">
-        <v>44</v>
-      </c>
-      <c r="B291" s="1">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2">
-      <c r="A292" t="s">
-        <v>45</v>
-      </c>
-      <c r="B292" s="1">
-        <v>1509</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2">
-      <c r="A293" t="s">
-        <v>46</v>
-      </c>
-      <c r="B293" s="1">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2">
-      <c r="A294" t="s">
-        <v>47</v>
-      </c>
-      <c r="B294" s="1">
-        <v>1683</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2">
-      <c r="A295" t="s">
-        <v>48</v>
-      </c>
-      <c r="B295" s="1">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2">
-      <c r="A296" t="s">
-        <v>49</v>
-      </c>
-      <c r="B296" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2">
-      <c r="A297" t="s">
-        <v>50</v>
-      </c>
-      <c r="B297" s="1">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2">
-      <c r="A298" t="s">
-        <v>51</v>
-      </c>
-      <c r="B298" s="1">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2">
-      <c r="A299" t="s">
-        <v>52</v>
-      </c>
-      <c r="B299" s="1">
-        <v>1729</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2">
-      <c r="A300" t="s">
-        <v>53</v>
-      </c>
-      <c r="B300" s="1">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2">
-      <c r="A301" t="s">
-        <v>54</v>
-      </c>
-      <c r="B301" s="1">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2">
-      <c r="A302" t="s">
-        <v>55</v>
-      </c>
-      <c r="B302" s="1">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2">
-      <c r="A303" t="s">
-        <v>56</v>
-      </c>
-      <c r="B303" s="1">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2">
-      <c r="A304" t="s">
-        <v>57</v>
-      </c>
-      <c r="B304" s="1">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2">
-      <c r="A305" t="s">
-        <v>58</v>
-      </c>
-      <c r="B305" s="1">
-        <v>1288</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2">
-      <c r="A306" t="s">
-        <v>59</v>
-      </c>
-      <c r="B306" s="1">
-        <v>1616</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2">
-      <c r="A307" t="s">
-        <v>60</v>
-      </c>
-      <c r="B307" s="1">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2">
-      <c r="A308" t="s">
-        <v>61</v>
-      </c>
-      <c r="B308" s="1">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2">
-      <c r="A309" t="s">
-        <v>62</v>
-      </c>
-      <c r="B309" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2">
-      <c r="A310" t="s">
-        <v>63</v>
-      </c>
-      <c r="B310" s="1">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2">
-      <c r="A311" t="s">
-        <v>64</v>
-      </c>
-      <c r="B311" s="1">
-        <v>1145</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2">
-      <c r="A312" t="s">
-        <v>65</v>
-      </c>
-      <c r="B312" s="1">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2">
-      <c r="A313" t="s">
-        <v>66</v>
-      </c>
-      <c r="B313" s="1">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2">
-      <c r="A314" t="s">
-        <v>67</v>
-      </c>
-      <c r="B314" s="1">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2">
-      <c r="A315" t="s">
-        <v>68</v>
-      </c>
-      <c r="B315" s="1">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2">
-      <c r="A316" t="s">
-        <v>69</v>
-      </c>
-      <c r="B316" s="1">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2">
-      <c r="A317" t="s">
-        <v>70</v>
-      </c>
-      <c r="B317" s="1">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2">
-      <c r="A318" t="s">
-        <v>71</v>
-      </c>
-      <c r="B318" s="1">
-        <v>1965</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2">
-      <c r="A319" t="s">
-        <v>72</v>
-      </c>
-      <c r="B319" s="1">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2">
-      <c r="A320" t="s">
-        <v>73</v>
-      </c>
-      <c r="B320" s="1">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2">
-      <c r="A321" t="s">
-        <v>74</v>
-      </c>
-      <c r="B321" s="1">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2">
-      <c r="A322" t="s">
-        <v>75</v>
-      </c>
-      <c r="B322" s="1">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2">
-      <c r="A323" t="s">
-        <v>76</v>
-      </c>
-      <c r="B323" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2">
-      <c r="A324" t="s">
-        <v>77</v>
-      </c>
-      <c r="B324" s="1">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2">
-      <c r="A325" t="s">
-        <v>78</v>
-      </c>
-      <c r="B325" s="1">
-        <v>1840</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2">
-      <c r="A326" t="s">
-        <v>79</v>
-      </c>
-      <c r="B326" s="1">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2">
-      <c r="A327" t="s">
-        <v>80</v>
-      </c>
-      <c r="B327" s="1">
-        <v>1902</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2">
-      <c r="A328" t="s">
-        <v>81</v>
-      </c>
-      <c r="B328" s="1">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2">
-      <c r="A329" t="s">
-        <v>82</v>
-      </c>
-      <c r="B329" s="1">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2">
-      <c r="A330" t="s">
-        <v>83</v>
-      </c>
-      <c r="B330" s="1">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2">
-      <c r="A331" t="s">
-        <v>84</v>
-      </c>
-      <c r="B331" s="1">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2">
-      <c r="A332" t="s">
-        <v>85</v>
-      </c>
-      <c r="B332" s="1">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2">
-      <c r="A333" t="s">
-        <v>86</v>
-      </c>
-      <c r="B333" s="1">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2">
-      <c r="A334" t="s">
-        <v>87</v>
-      </c>
-      <c r="B334" s="1">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2">
-      <c r="A335" t="s">
-        <v>88</v>
-      </c>
-      <c r="B335" s="1">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2">
-      <c r="A336" t="s">
-        <v>89</v>
-      </c>
-      <c r="B336" s="1">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2">
-      <c r="A337" t="s">
-        <v>90</v>
-      </c>
-      <c r="B337" s="1">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="338" spans="1:2">
-      <c r="A338" t="s">
-        <v>91</v>
-      </c>
-      <c r="B338" s="1">
-        <v>1672</v>
-      </c>
-    </row>
-    <row r="339" spans="1:2">
-      <c r="A339" t="s">
-        <v>92</v>
-      </c>
-      <c r="B339" s="1">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="340" spans="1:2">
-      <c r="A340" t="s">
-        <v>93</v>
-      </c>
-      <c r="B340" s="1">
-        <v>1556</v>
-      </c>
-    </row>
-    <row r="341" spans="1:2">
-      <c r="A341" t="s">
-        <v>94</v>
-      </c>
-      <c r="B341" s="1">
-        <v>1825</v>
-      </c>
-    </row>
-    <row r="342" spans="1:2">
-      <c r="A342" t="s">
-        <v>95</v>
-      </c>
-      <c r="B342" s="1">
-        <v>1801</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2">
-      <c r="A343" t="s">
-        <v>96</v>
-      </c>
-      <c r="B343" s="1">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2">
-      <c r="A344" t="s">
-        <v>97</v>
-      </c>
-      <c r="B344" s="1">
-        <v>1203</v>
-      </c>
-    </row>
-    <row r="345" spans="1:2">
-      <c r="A345" t="s">
-        <v>98</v>
-      </c>
-      <c r="B345" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="346" spans="1:2">
-      <c r="A346" t="s">
-        <v>99</v>
-      </c>
-      <c r="B346" s="1">
-        <v>1670</v>
-      </c>
-    </row>
-    <row r="347" spans="1:2">
-      <c r="A347" t="s">
-        <v>100</v>
-      </c>
-      <c r="B347" s="1">
-        <v>1741</v>
-      </c>
-    </row>
-    <row r="348" spans="1:2">
-      <c r="A348" t="s">
-        <v>101</v>
-      </c>
-      <c r="B348" s="1">
-        <v>1968</v>
-      </c>
-    </row>
-    <row r="349" spans="1:2">
-      <c r="A349" t="s">
-        <v>102</v>
-      </c>
-      <c r="B349" s="1">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2">
-      <c r="A350" t="s">
-        <v>103</v>
-      </c>
-      <c r="B350" s="1">
-        <v>1616</v>
-      </c>
-    </row>
-    <row r="351" spans="1:2">
-      <c r="A351" t="s">
-        <v>104</v>
-      </c>
-      <c r="B351" s="1">
-        <v>1638</v>
-      </c>
-    </row>
-    <row r="352" spans="1:2">
-      <c r="A352" t="s">
-        <v>105</v>
-      </c>
-      <c r="B352" s="1">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="353" spans="1:2">
-      <c r="A353" t="s">
-        <v>106</v>
-      </c>
-      <c r="B353" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="354" spans="1:2">
-      <c r="A354" t="s">
-        <v>107</v>
-      </c>
-      <c r="B354" s="1">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="355" spans="1:2">
-      <c r="A355" t="s">
-        <v>108</v>
-      </c>
-      <c r="B355" s="1">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="356" spans="1:2">
-      <c r="A356" t="s">
-        <v>109</v>
-      </c>
-      <c r="B356" s="1">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="357" spans="1:2">
-      <c r="A357" t="s">
-        <v>110</v>
-      </c>
-      <c r="B357" s="1">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="358" spans="1:2">
-      <c r="A358" t="s">
-        <v>111</v>
-      </c>
-      <c r="B358" s="1">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="359" spans="1:2">
-      <c r="A359" t="s">
-        <v>112</v>
-      </c>
-      <c r="B359" s="1">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="360" spans="1:2">
-      <c r="A360" t="s">
-        <v>113</v>
-      </c>
-      <c r="B360" s="1">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="361" spans="1:2">
-      <c r="A361" t="s">
-        <v>114</v>
-      </c>
-      <c r="B361" s="1">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2">
-      <c r="A362" t="s">
-        <v>115</v>
-      </c>
-      <c r="B362" s="1">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="363" spans="1:2">
-      <c r="A363" t="s">
-        <v>116</v>
-      </c>
-      <c r="B363" s="1">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="364" spans="1:2">
-      <c r="A364" t="s">
-        <v>117</v>
-      </c>
-      <c r="B364" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="365" spans="1:2">
-      <c r="A365" t="s">
-        <v>118</v>
-      </c>
-      <c r="B365" s="1">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="366" spans="1:2">
-      <c r="A366" t="s">
-        <v>119</v>
-      </c>
-      <c r="B366" s="1">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2">
-      <c r="A367" t="s">
-        <v>120</v>
-      </c>
-      <c r="B367" s="1">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="368" spans="1:2">
-      <c r="A368" t="s">
-        <v>121</v>
-      </c>
-      <c r="B368" s="1">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="369" spans="1:2">
-      <c r="A369" t="s">
-        <v>122</v>
-      </c>
-      <c r="B369" s="1">
-        <v>1647</v>
-      </c>
-    </row>
-    <row r="370" spans="1:2">
-      <c r="A370" t="s">
-        <v>123</v>
-      </c>
-      <c r="B370" s="1">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="371" spans="1:2">
-      <c r="A371" t="s">
-        <v>124</v>
-      </c>
-      <c r="B371" s="1">
-        <v>1988</v>
-      </c>
-    </row>
-    <row r="372" spans="1:2">
-      <c r="A372" t="s">
-        <v>125</v>
-      </c>
-      <c r="B372" s="1">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="373" spans="1:2">
-      <c r="A373" t="s">
-        <v>126</v>
-      </c>
-      <c r="B373" s="1">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="374" spans="1:2">
-      <c r="A374" t="s">
-        <v>127</v>
-      </c>
-      <c r="B374" s="1">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="375" spans="1:2">
-      <c r="A375" t="s">
-        <v>128</v>
-      </c>
-      <c r="B375" s="1">
-        <v>1899</v>
-      </c>
-    </row>
-    <row r="376" spans="1:2">
-      <c r="A376" t="s">
-        <v>129</v>
-      </c>
-      <c r="B376" s="1">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="377" spans="1:2">
-      <c r="A377" t="s">
-        <v>130</v>
-      </c>
-      <c r="B377" s="1">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="378" spans="1:2">
-      <c r="A378" t="s">
-        <v>131</v>
-      </c>
-      <c r="B378" s="1">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="379" spans="1:2">
-      <c r="A379" t="s">
-        <v>132</v>
-      </c>
-      <c r="B379" s="1">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="380" spans="1:2">
-      <c r="A380" t="s">
-        <v>133</v>
-      </c>
-      <c r="B380" s="1">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="381" spans="1:2">
-      <c r="A381" t="s">
-        <v>134</v>
-      </c>
-      <c r="B381" s="1">
-        <v>1549</v>
-      </c>
-    </row>
-    <row r="382" spans="1:2">
-      <c r="A382" t="s">
-        <v>135</v>
-      </c>
-      <c r="B382" s="1">
-        <v>1701</v>
-      </c>
-    </row>
-    <row r="383" spans="1:2">
-      <c r="A383" t="s">
-        <v>136</v>
-      </c>
-      <c r="B383" s="1">
-        <v>1152</v>
-      </c>
-    </row>
-    <row r="384" spans="1:2">
-      <c r="A384" t="s">
-        <v>137</v>
-      </c>
-      <c r="B384" s="1">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2">
-      <c r="A385" t="s">
-        <v>138</v>
-      </c>
-      <c r="B385" s="1">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="386" spans="1:2">
-      <c r="A386" t="s">
-        <v>139</v>
-      </c>
-      <c r="B386" s="1">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="387" spans="1:2">
-      <c r="A387" t="s">
-        <v>140</v>
-      </c>
-      <c r="B387" s="1">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="388" spans="1:2">
-      <c r="A388" t="s">
-        <v>141</v>
-      </c>
-      <c r="B388" s="1">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="389" spans="1:2">
-      <c r="A389" t="s">
-        <v>142</v>
-      </c>
-      <c r="B389" s="1">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="390" spans="1:2">
-      <c r="A390" t="s">
-        <v>143</v>
-      </c>
-      <c r="B390" s="1">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="391" spans="1:2">
-      <c r="A391" t="s">
-        <v>144</v>
-      </c>
-      <c r="B391" s="1">
-        <v>1615</v>
-      </c>
-    </row>
-    <row r="392" spans="1:2">
-      <c r="A392" t="s">
-        <v>145</v>
-      </c>
-      <c r="B392" s="1">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="393" spans="1:2">
-      <c r="A393" t="s">
-        <v>146</v>
-      </c>
-      <c r="B393" s="1">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="394" spans="1:2">
-      <c r="A394" t="s">
-        <v>147</v>
-      </c>
-      <c r="B394" s="1">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="395" spans="1:2">
-      <c r="A395" t="s">
-        <v>148</v>
-      </c>
-      <c r="B395" s="1">
-        <v>1852</v>
-      </c>
-    </row>
-    <row r="396" spans="1:2">
-      <c r="A396" t="s">
-        <v>149</v>
-      </c>
-      <c r="B396" s="1">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="397" spans="1:2">
-      <c r="A397" t="s">
-        <v>150</v>
-      </c>
-      <c r="B397" s="1">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="398" spans="1:2">
-      <c r="A398" t="s">
-        <v>151</v>
-      </c>
-      <c r="B398" s="1">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="399" spans="1:2">
-      <c r="A399" t="s">
-        <v>152</v>
-      </c>
-      <c r="B399" s="1">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="400" spans="1:2">
-      <c r="A400" t="s">
-        <v>153</v>
-      </c>
-      <c r="B400" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2">
-      <c r="A401" t="s">
-        <v>154</v>
-      </c>
-      <c r="B401" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="402" spans="1:2">
-      <c r="A402" t="s">
-        <v>155</v>
-      </c>
-      <c r="B402" s="1">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="403" spans="1:2">
-      <c r="A403" t="s">
-        <v>156</v>
-      </c>
-      <c r="B403" s="1">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="404" spans="1:2">
-      <c r="A404" t="s">
-        <v>157</v>
-      </c>
-      <c r="B404" s="1">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="405" spans="1:2">
-      <c r="A405" t="s">
-        <v>158</v>
-      </c>
-      <c r="B405" s="1">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="406" spans="1:2">
-      <c r="A406" t="s">
-        <v>159</v>
-      </c>
-      <c r="B406" s="1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="407" spans="1:2">
-      <c r="A407" t="s">
-        <v>160</v>
-      </c>
-      <c r="B407" s="1">
-        <v>1806</v>
-      </c>
-    </row>
-    <row r="408" spans="1:2">
-      <c r="A408" t="s">
-        <v>161</v>
-      </c>
-      <c r="B408" s="1">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="409" spans="1:2">
-      <c r="A409" t="s">
-        <v>162</v>
-      </c>
-      <c r="B409" s="1">
-        <v>1705</v>
-      </c>
-    </row>
-    <row r="410" spans="1:2">
-      <c r="A410" t="s">
-        <v>163</v>
-      </c>
-      <c r="B410" s="1">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="411" spans="1:2">
-      <c r="A411" t="s">
-        <v>164</v>
-      </c>
-      <c r="B411" s="1">
-        <v>1398</v>
-      </c>
-    </row>
-    <row r="412" spans="1:2">
-      <c r="A412" t="s">
-        <v>165</v>
-      </c>
-      <c r="B412" s="1">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="413" spans="1:2">
-      <c r="A413" t="s">
-        <v>166</v>
-      </c>
-      <c r="B413" s="1">
-        <v>1468</v>
-      </c>
-    </row>
-    <row r="414" spans="1:2">
-      <c r="A414" t="s">
-        <v>167</v>
-      </c>
-      <c r="B414" s="1">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="415" spans="1:2">
-      <c r="A415" t="s">
-        <v>168</v>
-      </c>
-      <c r="B415" s="1">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="416" spans="1:2">
-      <c r="A416" t="s">
-        <v>169</v>
-      </c>
-      <c r="B416" s="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="417" spans="1:2">
-      <c r="A417" t="s">
-        <v>170</v>
-      </c>
-      <c r="B417" s="1">
-        <v>1935</v>
-      </c>
-    </row>
-    <row r="418" spans="1:2">
-      <c r="A418" t="s">
-        <v>171</v>
-      </c>
-      <c r="B418" s="1">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="419" spans="1:2">
-      <c r="A419" t="s">
-        <v>172</v>
-      </c>
-      <c r="B419" s="1">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="420" spans="1:2">
-      <c r="A420" t="s">
-        <v>173</v>
-      </c>
-      <c r="B420" s="1">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="421" spans="1:2">
-      <c r="A421" t="s">
-        <v>174</v>
-      </c>
-      <c r="B421" s="1">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="422" spans="1:2">
-      <c r="A422" t="s">
-        <v>175</v>
-      </c>
-      <c r="B422" s="1">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="423" spans="1:2">
-      <c r="A423" t="s">
-        <v>176</v>
-      </c>
-      <c r="B423" s="1">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="424" spans="1:2">
-      <c r="A424" t="s">
-        <v>177</v>
-      </c>
-      <c r="B424" s="1">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="425" spans="1:2">
-      <c r="A425" t="s">
-        <v>178</v>
-      </c>
-      <c r="B425" s="1">
-        <v>1647</v>
-      </c>
-    </row>
-    <row r="426" spans="1:2">
-      <c r="A426" t="s">
-        <v>179</v>
-      </c>
-      <c r="B426" s="1">
-        <v>1822</v>
-      </c>
-    </row>
-    <row r="427" spans="1:2">
-      <c r="A427" t="s">
-        <v>180</v>
-      </c>
-      <c r="B427" s="1">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="428" spans="1:2">
-      <c r="A428" t="s">
-        <v>181</v>
-      </c>
-      <c r="B428" s="1">
-        <v>1686</v>
-      </c>
-    </row>
-    <row r="429" spans="1:2">
-      <c r="A429" t="s">
-        <v>182</v>
-      </c>
-      <c r="B429" s="1">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="430" spans="1:2">
-      <c r="A430" t="s">
-        <v>183</v>
-      </c>
-      <c r="B430" s="1">
-        <v>1975</v>
-      </c>
-    </row>
-    <row r="431" spans="1:2">
-      <c r="A431" t="s">
-        <v>184</v>
-      </c>
-      <c r="B431" s="1">
-        <v>1982</v>
-      </c>
-    </row>
-    <row r="432" spans="1:2">
-      <c r="A432" t="s">
-        <v>185</v>
-      </c>
-      <c r="B432" s="1">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="433" spans="1:2">
-      <c r="A433" t="s">
-        <v>186</v>
-      </c>
-      <c r="B433" s="1">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="434" spans="1:2">
-      <c r="A434" t="s">
-        <v>187</v>
-      </c>
-      <c r="B434" s="1">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="435" spans="1:2">
-      <c r="A435" t="s">
-        <v>188</v>
-      </c>
-      <c r="B435" s="1">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="436" spans="1:2">
-      <c r="A436" t="s">
-        <v>189</v>
-      </c>
-      <c r="B436" s="1">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="437" spans="1:2">
-      <c r="A437" t="s">
-        <v>190</v>
-      </c>
-      <c r="B437" s="1">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="438" spans="1:2">
-      <c r="A438" t="s">
-        <v>191</v>
-      </c>
-      <c r="B438" s="1">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="439" spans="1:2">
-      <c r="A439" t="s">
-        <v>192</v>
-      </c>
-      <c r="B439" s="1">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="440" spans="1:2">
-      <c r="A440" t="s">
-        <v>193</v>
-      </c>
-      <c r="B440" s="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="441" spans="1:2">
-      <c r="A441" t="s">
-        <v>194</v>
-      </c>
-      <c r="B441" s="1">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="442" spans="1:2">
-      <c r="A442" t="s">
-        <v>195</v>
-      </c>
-      <c r="B442" s="1">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="443" spans="1:2">
-      <c r="A443" t="s">
-        <v>196</v>
-      </c>
-      <c r="B443" s="1">
-        <v>1495</v>
-      </c>
-    </row>
-    <row r="444" spans="1:2">
-      <c r="A444" t="s">
-        <v>197</v>
-      </c>
-      <c r="B444" s="1">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="445" spans="1:2">
-      <c r="A445" t="s">
-        <v>198</v>
-      </c>
-      <c r="B445" s="1">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2">
-      <c r="A446" t="s">
-        <v>199</v>
-      </c>
-      <c r="B446" s="1">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="447" spans="1:2">
-      <c r="A447" t="s">
-        <v>200</v>
-      </c>
-      <c r="B447" s="1">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="448" spans="1:2">
-      <c r="A448" t="s">
-        <v>201</v>
-      </c>
-      <c r="B448" s="1">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="449" spans="1:2">
-      <c r="A449" t="s">
-        <v>202</v>
-      </c>
-      <c r="B449" s="1">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="450" spans="1:2">
-      <c r="A450" t="s">
-        <v>203</v>
-      </c>
-      <c r="B450" s="1">
-        <v>1369</v>
-      </c>
-    </row>
-    <row r="451" spans="1:2">
-      <c r="A451" t="s">
-        <v>204</v>
-      </c>
-      <c r="B451" s="1">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="452" spans="1:2">
-      <c r="A452" t="s">
-        <v>205</v>
-      </c>
-      <c r="B452" s="1">
-        <v>1852</v>
-      </c>
-    </row>
-    <row r="453" spans="1:2">
-      <c r="A453" t="s">
-        <v>206</v>
-      </c>
-      <c r="B453" s="1">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="454" spans="1:2">
-      <c r="A454" t="s">
-        <v>207</v>
-      </c>
-      <c r="B454" s="1">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="455" spans="1:2">
-      <c r="A455" t="s">
-        <v>208</v>
-      </c>
-      <c r="B455" s="1">
-        <v>1915</v>
-      </c>
-    </row>
-    <row r="456" spans="1:2">
-      <c r="A456" t="s">
-        <v>209</v>
-      </c>
-      <c r="B456" s="1">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="457" spans="1:2">
-      <c r="A457" t="s">
-        <v>210</v>
-      </c>
-      <c r="B457" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="458" spans="1:2">
-      <c r="A458" t="s">
-        <v>211</v>
-      </c>
-      <c r="B458" s="1">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="459" spans="1:2">
-      <c r="A459" t="s">
-        <v>212</v>
-      </c>
-      <c r="B459" s="1">
-        <v>1442</v>
-      </c>
-    </row>
-    <row r="460" spans="1:2">
-      <c r="A460" t="s">
-        <v>213</v>
-      </c>
-      <c r="B460" s="1">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="461" spans="1:2">
-      <c r="A461" t="s">
-        <v>214</v>
-      </c>
-      <c r="B461" s="1">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="462" spans="1:2">
-      <c r="A462" t="s">
-        <v>215</v>
-      </c>
-      <c r="B462" s="1">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="463" spans="1:2">
-      <c r="A463" t="s">
-        <v>216</v>
-      </c>
-      <c r="B463" s="1">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="464" spans="1:2">
-      <c r="A464" t="s">
-        <v>217</v>
-      </c>
-      <c r="B464" s="1">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="465" spans="1:2">
-      <c r="A465" t="s">
-        <v>218</v>
-      </c>
-      <c r="B465" s="1">
-        <v>1554</v>
-      </c>
-    </row>
-    <row r="466" spans="1:2">
-      <c r="A466" t="s">
-        <v>219</v>
-      </c>
-      <c r="B466" s="1">
-        <v>1369</v>
-      </c>
-    </row>
-    <row r="467" spans="1:2">
-      <c r="A467" t="s">
-        <v>220</v>
-      </c>
-      <c r="B467" s="1">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="468" spans="1:2">
-      <c r="A468" t="s">
-        <v>221</v>
-      </c>
-      <c r="B468" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="469" spans="1:2">
-      <c r="A469" t="s">
-        <v>222</v>
-      </c>
-      <c r="B469" s="1">
-        <v>1906</v>
-      </c>
-    </row>
-    <row r="470" spans="1:2">
-      <c r="A470" t="s">
-        <v>223</v>
-      </c>
-      <c r="B470" s="1">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="471" spans="1:2">
-      <c r="A471" t="s">
-        <v>224</v>
-      </c>
-      <c r="B471" s="1">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="472" spans="1:2">
-      <c r="A472" t="s">
-        <v>225</v>
-      </c>
-      <c r="B472" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="473" spans="1:2">
-      <c r="A473" t="s">
-        <v>226</v>
-      </c>
-      <c r="B473" s="1">
-        <v>1958</v>
-      </c>
-    </row>
-    <row r="474" spans="1:2">
-      <c r="A474" t="s">
-        <v>227</v>
-      </c>
-      <c r="B474" s="1">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="475" spans="1:2">
-      <c r="A475" t="s">
-        <v>228</v>
-      </c>
-      <c r="B475" s="1">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="476" spans="1:2">
-      <c r="A476" t="s">
-        <v>229</v>
-      </c>
-      <c r="B476" s="1">
-        <v>1378</v>
-      </c>
-    </row>
-    <row r="477" spans="1:2">
-      <c r="A477" t="s">
-        <v>230</v>
-      </c>
-      <c r="B477" s="1">
-        <v>1992</v>
-      </c>
-    </row>
-    <row r="478" spans="1:2">
-      <c r="A478" t="s">
-        <v>231</v>
-      </c>
-      <c r="B478" s="1">
-        <v>1920</v>
-      </c>
-    </row>
-    <row r="479" spans="1:2">
-      <c r="A479" t="s">
-        <v>232</v>
-      </c>
-      <c r="B479" s="1">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="480" spans="1:2">
-      <c r="A480" t="s">
-        <v>233</v>
-      </c>
-      <c r="B480" s="1">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="481" spans="1:2">
-      <c r="A481" t="s">
-        <v>234</v>
-      </c>
-      <c r="B481" s="1">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="482" spans="1:2">
-      <c r="A482" t="s">
-        <v>235</v>
-      </c>
-      <c r="B482" s="1">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="483" spans="1:2">
-      <c r="A483" t="s">
-        <v>236</v>
-      </c>
-      <c r="B483" s="1">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="484" spans="1:2">
-      <c r="A484" t="s">
-        <v>237</v>
-      </c>
-      <c r="B484" s="1">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="485" spans="1:2">
-      <c r="A485" t="s">
-        <v>238</v>
-      </c>
-      <c r="B485" s="1">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="486" spans="1:2">
-      <c r="A486" t="s">
-        <v>239</v>
-      </c>
-      <c r="B486" s="1">
-        <v>1905</v>
-      </c>
-    </row>
-    <row r="487" spans="1:2">
-      <c r="A487" t="s">
-        <v>240</v>
-      </c>
-      <c r="B487" s="1">
-        <v>1964</v>
-      </c>
-    </row>
-    <row r="488" spans="1:2">
-      <c r="A488" t="s">
-        <v>241</v>
-      </c>
-      <c r="B488" s="1">
-        <v>1470</v>
-      </c>
-    </row>
-    <row r="489" spans="1:2">
-      <c r="A489" t="s">
-        <v>242</v>
-      </c>
-      <c r="B489" s="1">
-        <v>1973</v>
-      </c>
-    </row>
-    <row r="490" spans="1:2">
-      <c r="A490" t="s">
-        <v>243</v>
-      </c>
-      <c r="B490" s="1">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="491" spans="1:2">
-      <c r="A491" t="s">
-        <v>244</v>
-      </c>
-      <c r="B491" s="1">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="492" spans="1:2">
-      <c r="A492" t="s">
-        <v>245</v>
-      </c>
-      <c r="B492" s="1">
-        <v>1937</v>
-      </c>
-    </row>
-    <row r="493" spans="1:2">
-      <c r="A493" t="s">
-        <v>246</v>
-      </c>
-      <c r="B493" s="1">
-        <v>1956</v>
-      </c>
-    </row>
-    <row r="494" spans="1:2">
-      <c r="A494" t="s">
-        <v>247</v>
-      </c>
-      <c r="B494" s="1">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="495" spans="1:2">
-      <c r="A495" t="s">
-        <v>248</v>
-      </c>
-      <c r="B495" s="1">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="496" spans="1:2">
-      <c r="A496" t="s">
-        <v>249</v>
-      </c>
-      <c r="B496" s="1">
-        <v>1661</v>
-      </c>
-    </row>
-    <row r="497" spans="1:2">
-      <c r="A497" t="s">
-        <v>250</v>
-      </c>
-      <c r="B497" s="1">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="498" spans="1:2">
-      <c r="A498" t="s">
-        <v>251</v>
-      </c>
-      <c r="B498" s="1">
         <v>1572</v>
       </c>
     </row>

</xml_diff>